<commit_message>
Add drill and construction uploader
</commit_message>
<xml_diff>
--- a/static/download_template/drilling_and_construction.xlsx
+++ b/static/download_template/drilling_and_construction.xlsx
@@ -77,7 +77,7 @@
 • No</t>
   </si>
   <si>
-    <t xml:space="preserve">Date as yyyy-mm-dd</t>
+    <t xml:space="preserve">Year as YYYY</t>
   </si>
   <si>
     <t xml:space="preserve">Installer (open text)</t>
@@ -295,12 +295,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -366,25 +366,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF953735"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="35.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="5" style="1" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="35.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="9" style="1" width="15.71"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -454,8 +454,8 @@
     <mergeCell ref="I1:J1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -464,7 +464,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF953735"/>
     <pageSetUpPr fitToPage="false"/>
@@ -472,15 +472,15 @@
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.71484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="19.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1019" min="5" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1020" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1019" min="5" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1020" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -532,8 +532,8 @@
     <mergeCell ref="B1:D1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -542,7 +542,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF953735"/>
     <pageSetUpPr fitToPage="false"/>
@@ -550,16 +550,16 @@
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.71484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="1" width="16.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="7" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1022" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="7" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -626,8 +626,8 @@
     <mergeCell ref="E1:F1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -636,7 +636,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF953735"/>
     <pageSetUpPr fitToPage="false"/>
@@ -644,15 +644,15 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="19.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="1" width="16.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="1" width="15.71"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -732,8 +732,8 @@
     <mergeCell ref="H1:I1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Add country to data provider/organisation (#128)
* Add country to data provider/organisation

* Change terms

* Change download file to ods

* Update uploader file to use ods

* Fix link
</commit_message>
<xml_diff>
--- a/static/download_template/drilling_and_construction.xlsx
+++ b/static/download_template/drilling_and_construction.xlsx
@@ -5,13 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Drilling and Construction" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Drilling" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Water Strike" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Stratigraphic Log" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Structures" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Construction" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -373,7 +373,7 @@
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -643,8 +643,8 @@
   </sheetPr>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Create script to read odf file effectively (#145)
* Create script to read odf file effectively

* Clean code

* Add tests

* Update the uploader

* Improved

* Update test to use uploader

* Add count

* Count on uploader

* Update uploader

* Fix stop/resume

---------

Co-authored-by: Irwan Fathurrahman <meomancer@gmail.com>
</commit_message>
<xml_diff>
--- a/static/download_template/drilling_and_construction.xlsx
+++ b/static/download_template/drilling_and_construction.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Drilling" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="35">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -123,6 +123,12 @@
     <t xml:space="preserve">Value (number)</t>
   </si>
   <si>
+    <t xml:space="preserve">Material: Open text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stratigraphic unit: Open text</t>
+  </si>
+  <si>
     <t xml:space="preserve">Type</t>
   </si>
   <si>
@@ -140,6 +146,9 @@
 • cm
 • ft
 • inch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description: Open text</t>
   </si>
 </sst>
 </file>
@@ -373,7 +382,7 @@
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -549,8 +558,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.71484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -611,10 +620,10 @@
         <v>10</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="AMH2" s="0"/>
       <c r="AMI2" s="0"/>
@@ -644,7 +653,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -660,7 +669,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>21</v>
@@ -678,7 +687,7 @@
         <v>3</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>3</v>
@@ -695,7 +704,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>26</v>
@@ -716,13 +725,13 @@
         <v>27</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update uploader with name column
</commit_message>
<xml_diff>
--- a/static/download_template/drilling_and_construction.xlsx
+++ b/static/download_template/drilling_and_construction.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Drilling" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,11 +23,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="37">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
   <si>
+    <t xml:space="preserve">Name </t>
+  </si>
+  <si>
     <t xml:space="preserve"> Total depth</t>
   </si>
   <si>
@@ -53,6 +56,9 @@
   </si>
   <si>
     <t xml:space="preserve">The original ID of the groundwater point.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The name of the data point.</t>
   </si>
   <si>
     <t xml:space="preserve">Unit must be either:
@@ -380,27 +386,29 @@
     <tabColor rgb="FF953735"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="35.7"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="5" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="35.7"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="9" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.62"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="35.7"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="35.7"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="1" width="15.71"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -418,49 +426,55 @@
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" s="6" customFormat="true" ht="159.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5"/>
       <c r="D2" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>14</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -481,34 +495,36 @@
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.71484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="19.62"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1019" min="5" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1020" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="1" width="19.62"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1020" min="6" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1021" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>17</v>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="AMF1" s="0"/>
+        <v>5</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
       <c r="AMI1" s="0"/>
@@ -516,21 +532,23 @@
     </row>
     <row r="2" s="6" customFormat="true" ht="159.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="AMF2" s="0"/>
+        <v>22</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="AMG2" s="0"/>
       <c r="AMH2" s="0"/>
       <c r="AMI2" s="0"/>
@@ -538,7 +556,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="C1:E1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -558,17 +576,17 @@
   </sheetPr>
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.71484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="1" width="16.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="7" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="19.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="1" width="16.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="8" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -576,63 +594,67 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>22</v>
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="AMH1" s="0"/>
+        <v>26</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" s="6" customFormat="true" ht="159.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="AMH2" s="0"/>
+        <v>30</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -650,18 +672,18 @@
     <tabColor rgb="FF953735"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="19.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="1" width="16.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="19.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="1" width="16.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="9" style="1" width="15.71"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -669,76 +691,82 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>22</v>
+        <v>32</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>18</v>
+        <v>26</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2" s="6" customFormat="true" ht="159.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Update uploader with name column (#150)
* Update uploader with name column

* Fix monitoring file for same original id not created

* Update download cache
</commit_message>
<xml_diff>
--- a/static/download_template/drilling_and_construction.xlsx
+++ b/static/download_template/drilling_and_construction.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Drilling" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,11 +23,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="37">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
   <si>
+    <t xml:space="preserve">Name </t>
+  </si>
+  <si>
     <t xml:space="preserve"> Total depth</t>
   </si>
   <si>
@@ -53,6 +56,9 @@
   </si>
   <si>
     <t xml:space="preserve">The original ID of the groundwater point.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The name of the data point.</t>
   </si>
   <si>
     <t xml:space="preserve">Unit must be either:
@@ -380,27 +386,29 @@
     <tabColor rgb="FF953735"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="35.7"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="5" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="35.7"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="9" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.62"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="35.7"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="35.7"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="1" width="15.71"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -418,49 +426,55 @@
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" s="6" customFormat="true" ht="159.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5"/>
       <c r="D2" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>14</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -481,34 +495,36 @@
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.71484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="19.62"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1019" min="5" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1020" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="1" width="19.62"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1020" min="6" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1021" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>17</v>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="AMF1" s="0"/>
+        <v>5</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
       <c r="AMI1" s="0"/>
@@ -516,21 +532,23 @@
     </row>
     <row r="2" s="6" customFormat="true" ht="159.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="AMF2" s="0"/>
+        <v>22</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="AMG2" s="0"/>
       <c r="AMH2" s="0"/>
       <c r="AMI2" s="0"/>
@@ -538,7 +556,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="C1:E1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -558,17 +576,17 @@
   </sheetPr>
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.71484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="1" width="16.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="7" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="19.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="1" width="16.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="8" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -576,63 +594,67 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>22</v>
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="AMH1" s="0"/>
+        <v>26</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" s="6" customFormat="true" ht="159.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="AMH2" s="0"/>
+        <v>30</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -650,18 +672,18 @@
     <tabColor rgb="FF953735"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="19.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="1" width="16.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="19.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="1" width="16.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="9" style="1" width="15.71"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -669,76 +691,82 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>22</v>
+        <v>32</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>18</v>
+        <v>26</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2" s="6" customFormat="true" ht="159.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>